<commit_message>
modification drivers mexico 29125
</commit_message>
<xml_diff>
--- a/ssp_modeling/transformations/templates/calibrated/mexico/model_input_variables_mexico_ip_calibrated.xlsx
+++ b/ssp_modeling/transformations/templates/calibrated/mexico/model_input_variables_mexico_ip_calibrated.xlsx
@@ -12815,109 +12815,109 @@
         <v>1</v>
       </c>
       <c r="J97">
-        <v>28.27747645785854</v>
+        <v>1</v>
       </c>
       <c r="K97">
-        <v>14.72694372729688</v>
+        <v>1</v>
       </c>
       <c r="L97">
-        <v>1.975943073368923</v>
+        <v>1</v>
       </c>
       <c r="M97">
-        <v>-4.982406736672811</v>
+        <v>1</v>
       </c>
       <c r="N97">
-        <v>13.71324098555475</v>
+        <v>1</v>
       </c>
       <c r="O97">
-        <v>0.5405825894773754</v>
+        <v>1</v>
       </c>
       <c r="P97">
-        <v>0.5558965031614629</v>
+        <v>1</v>
       </c>
       <c r="Q97">
-        <v>0.5712104168455503</v>
+        <v>1</v>
       </c>
       <c r="R97">
-        <v>0.5865243305296378</v>
+        <v>1</v>
       </c>
       <c r="S97">
-        <v>0.6018382442137253</v>
+        <v>1</v>
       </c>
       <c r="T97">
-        <v>0.6171521578978127</v>
+        <v>1</v>
       </c>
       <c r="U97">
-        <v>0.6324660715819003</v>
+        <v>1</v>
       </c>
       <c r="V97">
-        <v>0.6477799852659878</v>
+        <v>1</v>
       </c>
       <c r="W97">
-        <v>0.6630938989500753</v>
+        <v>1</v>
       </c>
       <c r="X97">
-        <v>0.6784078126341627</v>
+        <v>1</v>
       </c>
       <c r="Y97">
-        <v>0.6937217263182502</v>
+        <v>1</v>
       </c>
       <c r="Z97">
-        <v>0.7090356400023378</v>
+        <v>1</v>
       </c>
       <c r="AA97">
-        <v>0.7243495536864253</v>
+        <v>1</v>
       </c>
       <c r="AB97">
-        <v>0.7396634673705127</v>
+        <v>1</v>
       </c>
       <c r="AC97">
-        <v>0.7549773810546002</v>
+        <v>1</v>
       </c>
       <c r="AD97">
-        <v>0.7702912947386877</v>
+        <v>1</v>
       </c>
       <c r="AE97">
-        <v>0.7856052084227751</v>
+        <v>1</v>
       </c>
       <c r="AF97">
-        <v>0.8009191221068627</v>
+        <v>1</v>
       </c>
       <c r="AG97">
-        <v>0.8162330357909502</v>
+        <v>1</v>
       </c>
       <c r="AH97">
-        <v>0.8315469494750376</v>
+        <v>1</v>
       </c>
       <c r="AI97">
-        <v>0.8468608631591251</v>
+        <v>1</v>
       </c>
       <c r="AJ97">
-        <v>0.8621747768432126</v>
+        <v>1</v>
       </c>
       <c r="AK97">
-        <v>0.8774886905273001</v>
+        <v>1</v>
       </c>
       <c r="AL97">
-        <v>0.8928026042113876</v>
+        <v>1</v>
       </c>
       <c r="AM97">
-        <v>0.9081165178954752</v>
+        <v>1</v>
       </c>
       <c r="AN97">
-        <v>0.9234304315795624</v>
+        <v>1</v>
       </c>
       <c r="AO97">
-        <v>0.93874434526365</v>
+        <v>1</v>
       </c>
       <c r="AP97">
-        <v>0.9540582589477375</v>
+        <v>1</v>
       </c>
       <c r="AQ97">
-        <v>0.969372172631825</v>
+        <v>1</v>
       </c>
       <c r="AR97">
-        <v>0.9846860863159126</v>
+        <v>1</v>
       </c>
       <c r="AS97">
         <v>1</v>
@@ -14401,109 +14401,109 @@
         <v>1</v>
       </c>
       <c r="J110">
-        <v>7.262124304710232</v>
+        <v>1</v>
       </c>
       <c r="K110">
-        <v>-26.83274798980316</v>
+        <v>1</v>
       </c>
       <c r="L110">
-        <v>52.29618652428636</v>
+        <v>1</v>
       </c>
       <c r="M110">
-        <v>6.210359160774604</v>
+        <v>1</v>
       </c>
       <c r="N110">
-        <v>-16.20853421904294</v>
+        <v>1</v>
       </c>
       <c r="O110">
-        <v>1.082201201844458</v>
+        <v>1</v>
       </c>
       <c r="P110">
-        <v>1.079461161782976</v>
+        <v>1</v>
       </c>
       <c r="Q110">
-        <v>1.076721121721494</v>
+        <v>1</v>
       </c>
       <c r="R110">
-        <v>1.073981081660012</v>
+        <v>1</v>
       </c>
       <c r="S110">
-        <v>1.071241041598531</v>
+        <v>1</v>
       </c>
       <c r="T110">
-        <v>1.068501001537049</v>
+        <v>1</v>
       </c>
       <c r="U110">
-        <v>1.065760961475566</v>
+        <v>1</v>
       </c>
       <c r="V110">
-        <v>1.063020921414085</v>
+        <v>1</v>
       </c>
       <c r="W110">
-        <v>1.060280881352603</v>
+        <v>1</v>
       </c>
       <c r="X110">
-        <v>1.057540841291121</v>
+        <v>1</v>
       </c>
       <c r="Y110">
-        <v>1.054800801229639</v>
+        <v>1</v>
       </c>
       <c r="Z110">
-        <v>1.052060761168157</v>
+        <v>1</v>
       </c>
       <c r="AA110">
-        <v>1.049320721106675</v>
+        <v>1</v>
       </c>
       <c r="AB110">
-        <v>1.046580681045193</v>
+        <v>1</v>
       </c>
       <c r="AC110">
-        <v>1.043840640983711</v>
+        <v>1</v>
       </c>
       <c r="AD110">
-        <v>1.041100600922229</v>
+        <v>1</v>
       </c>
       <c r="AE110">
-        <v>1.038360560860747</v>
+        <v>1</v>
       </c>
       <c r="AF110">
-        <v>1.035620520799265</v>
+        <v>1</v>
       </c>
       <c r="AG110">
-        <v>1.032880480737783</v>
+        <v>1</v>
       </c>
       <c r="AH110">
-        <v>1.030140440676301</v>
+        <v>1</v>
       </c>
       <c r="AI110">
-        <v>1.027400400614819</v>
+        <v>1</v>
       </c>
       <c r="AJ110">
-        <v>1.024660360553338</v>
+        <v>1</v>
       </c>
       <c r="AK110">
-        <v>1.021920320491855</v>
+        <v>1</v>
       </c>
       <c r="AL110">
-        <v>1.019180280430374</v>
+        <v>1</v>
       </c>
       <c r="AM110">
-        <v>1.016440240368892</v>
+        <v>1</v>
       </c>
       <c r="AN110">
-        <v>1.01370020030741</v>
+        <v>1</v>
       </c>
       <c r="AO110">
-        <v>1.010960160245927</v>
+        <v>1</v>
       </c>
       <c r="AP110">
-        <v>1.008220120184446</v>
+        <v>1</v>
       </c>
       <c r="AQ110">
-        <v>1.005480080122964</v>
+        <v>1</v>
       </c>
       <c r="AR110">
-        <v>1.002740040061482</v>
+        <v>1</v>
       </c>
       <c r="AS110">
         <v>1</v>
@@ -17085,112 +17085,112 @@
         <v>1</v>
       </c>
       <c r="J132">
-        <v>46350000</v>
+        <v>34994250</v>
       </c>
       <c r="K132">
-        <v>47720000</v>
+        <v>36028600</v>
       </c>
       <c r="L132">
-        <v>48360000</v>
+        <v>36511800</v>
       </c>
       <c r="M132">
-        <v>48330000</v>
+        <v>36489150</v>
       </c>
       <c r="N132">
-        <v>45160000</v>
+        <v>34095800</v>
       </c>
       <c r="O132">
-        <v>47830000</v>
+        <v>36111650</v>
       </c>
       <c r="P132">
-        <v>48786600</v>
+        <v>36833883</v>
       </c>
       <c r="Q132">
-        <v>49762332</v>
+        <v>37570560.66</v>
       </c>
       <c r="R132">
-        <v>50757578.64</v>
+        <v>38321971.8732</v>
       </c>
       <c r="S132">
-        <v>51772730.21</v>
+        <v>39088411.30855</v>
       </c>
       <c r="T132">
-        <v>52808184.82</v>
+        <v>39870179.5391</v>
       </c>
       <c r="U132">
-        <v>53864348.51</v>
+        <v>40667583.12505</v>
       </c>
       <c r="V132">
-        <v>54941635.48</v>
+        <v>41480934.7874</v>
       </c>
       <c r="W132">
-        <v>56040468.19</v>
+        <v>42310553.48345</v>
       </c>
       <c r="X132">
-        <v>57161277.56</v>
+        <v>43156764.5578</v>
       </c>
       <c r="Y132">
-        <v>58304503.11</v>
+        <v>44019899.84805</v>
       </c>
       <c r="Z132">
-        <v>59470593.17</v>
+        <v>44900297.84335</v>
       </c>
       <c r="AA132">
-        <v>60660005.03</v>
+        <v>45798303.79765</v>
       </c>
       <c r="AB132">
-        <v>61873205.13</v>
+        <v>46714269.87315001</v>
       </c>
       <c r="AC132">
-        <v>63110669.24</v>
+        <v>47648555.2762</v>
       </c>
       <c r="AD132">
-        <v>64372882.62</v>
+        <v>48601526.3781</v>
       </c>
       <c r="AE132">
-        <v>65660340.27</v>
+        <v>49573556.90385</v>
       </c>
       <c r="AF132">
-        <v>66973547.08</v>
+        <v>50565028.0454</v>
       </c>
       <c r="AG132">
-        <v>68313018.02</v>
+        <v>51576328.6051</v>
       </c>
       <c r="AH132">
-        <v>69679278.38</v>
+        <v>52607855.1769</v>
       </c>
       <c r="AI132">
-        <v>71072863.95</v>
+        <v>53660012.28225</v>
       </c>
       <c r="AJ132">
-        <v>72494321.23</v>
+        <v>54733212.52865</v>
       </c>
       <c r="AK132">
-        <v>73944207.65000001</v>
+        <v>55827876.77575</v>
       </c>
       <c r="AL132">
-        <v>75423091.81</v>
+        <v>56944434.31655</v>
       </c>
       <c r="AM132">
-        <v>76931553.64</v>
+        <v>58083322.9982</v>
       </c>
       <c r="AN132">
-        <v>78470184.72</v>
+        <v>59244989.4636</v>
       </c>
       <c r="AO132">
-        <v>80039588.41</v>
+        <v>60429889.24955</v>
       </c>
       <c r="AP132">
-        <v>81640380.18000001</v>
+        <v>61638487.0359</v>
       </c>
       <c r="AQ132">
-        <v>83273187.78</v>
+        <v>62871256.7739</v>
       </c>
       <c r="AR132">
-        <v>84938651.54000001</v>
+        <v>64128681.9127</v>
       </c>
       <c r="AS132">
-        <v>86637424.56999999</v>
+        <v>65411255.55035</v>
       </c>
     </row>
     <row r="133" spans="1:45">
@@ -17329,112 +17329,112 @@
         <v>1</v>
       </c>
       <c r="J134">
-        <v>13405879.2513089</v>
+        <v>268117.585026178</v>
       </c>
       <c r="K134">
-        <v>12428766.4964308</v>
+        <v>248575.329928616</v>
       </c>
       <c r="L134">
-        <v>13740508.525777</v>
+        <v>274810.17051554</v>
       </c>
       <c r="M134">
-        <v>13914594.2001128</v>
+        <v>278291.884002256</v>
       </c>
       <c r="N134">
-        <v>14624116.213285</v>
+        <v>292482.3242657</v>
       </c>
       <c r="O134">
-        <v>12996545.3379814</v>
+        <v>259930.906759628</v>
       </c>
       <c r="P134">
-        <v>12996550</v>
+        <v>259931</v>
       </c>
       <c r="Q134">
-        <v>13065804.1181437</v>
+        <v>261316.082362874</v>
       </c>
       <c r="R134">
-        <v>13135427.2675211</v>
+        <v>262708.545350422</v>
       </c>
       <c r="S134">
-        <v>13205421.4145718</v>
+        <v>264108.428291436</v>
       </c>
       <c r="T134">
-        <v>13275788.5362143</v>
+        <v>265515.770724286</v>
       </c>
       <c r="U134">
-        <v>13346530.6199009</v>
+        <v>266930.612398018</v>
       </c>
       <c r="V134">
-        <v>13417649.6636748</v>
+        <v>268352.993273496</v>
       </c>
       <c r="W134">
-        <v>13489147.6762257</v>
+        <v>269782.953524514</v>
       </c>
       <c r="X134">
-        <v>13561026.6769472</v>
+        <v>271220.533538944</v>
       </c>
       <c r="Y134">
-        <v>13633288.6959935</v>
+        <v>272665.77391987</v>
       </c>
       <c r="Z134">
-        <v>13705935.7743365</v>
+        <v>274118.71548673</v>
       </c>
       <c r="AA134">
-        <v>13778969.9638242</v>
+        <v>275579.399276484</v>
       </c>
       <c r="AB134">
-        <v>13852393.3272378</v>
+        <v>277047.866544756</v>
       </c>
       <c r="AC134">
-        <v>13926207.9383506</v>
+        <v>278524.158767012</v>
       </c>
       <c r="AD134">
-        <v>14000415.8819861</v>
+        <v>280008.317639722</v>
       </c>
       <c r="AE134">
-        <v>14075019.2540773</v>
+        <v>281500.385081546</v>
       </c>
       <c r="AF134">
-        <v>14150020.1617256</v>
+        <v>283000.403234512</v>
       </c>
       <c r="AG134">
-        <v>14225420.7232605</v>
+        <v>284508.41446521</v>
       </c>
       <c r="AH134">
-        <v>14301223.0682991</v>
+        <v>286024.461365982</v>
       </c>
       <c r="AI134">
-        <v>14377429.3378069</v>
+        <v>287548.586756138</v>
       </c>
       <c r="AJ134">
-        <v>14454041.6841575</v>
+        <v>289080.83368315</v>
       </c>
       <c r="AK134">
-        <v>14531062.271194</v>
+        <v>290621.24542388</v>
       </c>
       <c r="AL134">
-        <v>14608493.2742896</v>
+        <v>292169.865485792</v>
       </c>
       <c r="AM134">
-        <v>14686336.8804097</v>
+        <v>293726.737608194</v>
       </c>
       <c r="AN134">
-        <v>14764595.2881728</v>
+        <v>295291.905763456</v>
       </c>
       <c r="AO134">
-        <v>14843270.7079135</v>
+        <v>296865.41415827</v>
       </c>
       <c r="AP134">
-        <v>14922365.3617443</v>
+        <v>298447.307234886</v>
       </c>
       <c r="AQ134">
-        <v>15001881.4836186</v>
+        <v>300037.629672372</v>
       </c>
       <c r="AR134">
-        <v>15081821.3193938</v>
+        <v>301636.426387876</v>
       </c>
       <c r="AS134">
-        <v>15162187.1268947</v>
+        <v>303243.742537894</v>
       </c>
     </row>
     <row r="135" spans="1:45">
@@ -17451,112 +17451,112 @@
         <v>1</v>
       </c>
       <c r="J135">
-        <v>545738.738287517</v>
+        <v>1091477.476575034</v>
       </c>
       <c r="K135">
-        <v>512507.04078475</v>
+        <v>1025014.0815695</v>
       </c>
       <c r="L135">
-        <v>504807.68549269</v>
+        <v>1009615.37098538</v>
       </c>
       <c r="M135">
-        <v>517800.477085705</v>
+        <v>1035600.95417141</v>
       </c>
       <c r="N135">
-        <v>528082.236764549</v>
+        <v>1056164.473529098</v>
       </c>
       <c r="O135">
-        <v>464580.939430365</v>
+        <v>929161.87886073</v>
       </c>
       <c r="P135">
-        <v>464580.9</v>
+        <v>929161.8</v>
       </c>
       <c r="Q135">
-        <v>454242.999773233</v>
+        <v>908485.999546466</v>
       </c>
       <c r="R135">
-        <v>444135.139526798</v>
+        <v>888270.279053596</v>
       </c>
       <c r="S135">
-        <v>434252.200388255</v>
+        <v>868504.40077651</v>
       </c>
       <c r="T135">
-        <v>424589.177390822</v>
+        <v>849178.354781644</v>
       </c>
       <c r="U135">
-        <v>415141.176938734</v>
+        <v>830282.353877468</v>
       </c>
       <c r="V135">
-        <v>405903.414329003</v>
+        <v>811806.828658006</v>
       </c>
       <c r="W135">
-        <v>396871.211328326</v>
+        <v>793742.4226566521</v>
       </c>
       <c r="X135">
-        <v>388039.993803911</v>
+        <v>776079.9876078221</v>
       </c>
       <c r="Y135">
-        <v>379405.289407023</v>
+        <v>758810.578814046</v>
       </c>
       <c r="Z135">
-        <v>370962.725308073</v>
+        <v>741925.450616146</v>
       </c>
       <c r="AA135">
-        <v>362708.025982112</v>
+        <v>725416.051964224</v>
       </c>
       <c r="AB135">
-        <v>354637.011043593</v>
+        <v>709274.022087186</v>
       </c>
       <c r="AC135">
-        <v>346745.593129323</v>
+        <v>693491.186258646</v>
       </c>
       <c r="AD135">
-        <v>339029.775828521</v>
+        <v>678059.551657042</v>
       </c>
       <c r="AE135">
-        <v>331485.651658934</v>
+        <v>662971.303317868</v>
       </c>
       <c r="AF135">
-        <v>324109.400087991</v>
+        <v>648218.8001759819</v>
       </c>
       <c r="AG135">
-        <v>316897.285597992</v>
+        <v>633794.571195984</v>
       </c>
       <c r="AH135">
-        <v>309845.655794344</v>
+        <v>619691.3115886881</v>
       </c>
       <c r="AI135">
-        <v>302950.939555904</v>
+        <v>605901.879111808</v>
       </c>
       <c r="AJ135">
-        <v>296209.645226468</v>
+        <v>592419.290452936</v>
       </c>
       <c r="AK135">
-        <v>289618.358846513</v>
+        <v>579236.7176930259</v>
       </c>
       <c r="AL135">
-        <v>283173.742424281</v>
+        <v>566347.484848562</v>
       </c>
       <c r="AM135">
-        <v>276872.532245338</v>
+        <v>553745.064490676</v>
       </c>
       <c r="AN135">
-        <v>270711.537219746</v>
+        <v>541423.074439492</v>
       </c>
       <c r="AO135">
-        <v>264687.637266019</v>
+        <v>529375.274532038</v>
       </c>
       <c r="AP135">
-        <v>258797.781731031</v>
+        <v>517595.563462062</v>
       </c>
       <c r="AQ135">
-        <v>253038.987845092</v>
+        <v>506077.975690184</v>
       </c>
       <c r="AR135">
-        <v>247408.339211399</v>
+        <v>494816.678422798</v>
       </c>
       <c r="AS135">
-        <v>241902.984329101</v>
+        <v>483805.968658202</v>
       </c>
     </row>
     <row r="136" spans="1:45">
@@ -17573,112 +17573,112 @@
         <v>1</v>
       </c>
       <c r="J136">
-        <v>18508.0363027602</v>
+        <v>37016.0726055204</v>
       </c>
       <c r="K136">
-        <v>25857.1604612335</v>
+        <v>51714.320922467</v>
       </c>
       <c r="L136">
-        <v>20575.5678991988</v>
+        <v>41151.1357983976</v>
       </c>
       <c r="M136">
-        <v>22002.8100351866</v>
+        <v>44005.6200703732</v>
       </c>
       <c r="N136">
-        <v>3892.74616461976</v>
+        <v>7785.49232923952</v>
       </c>
       <c r="O136">
-        <v>21032.9471766494</v>
+        <v>42065.8943532988</v>
       </c>
       <c r="P136">
-        <v>21032.95</v>
+        <v>42065.9</v>
       </c>
       <c r="Q136">
-        <v>65835.2597840144</v>
+        <v>131670.5195680288</v>
       </c>
       <c r="R136">
-        <v>206071.018607882</v>
+        <v>412142.037215764</v>
       </c>
       <c r="S136">
-        <v>645023.120580156</v>
+        <v>1290046.241160312</v>
       </c>
       <c r="T136">
-        <v>2018987.57473822</v>
+        <v>4037975.14947644</v>
       </c>
       <c r="U136">
-        <v>6319635.21444151</v>
+        <v>12639270.42888302</v>
       </c>
       <c r="V136">
-        <v>19781097.0920847</v>
+        <v>39562194.1841694</v>
       </c>
       <c r="W136">
-        <v>61916833.6286733</v>
+        <v>123833667.2573466</v>
       </c>
       <c r="X136">
-        <v>193805948.616209</v>
+        <v>387611897.232418</v>
       </c>
       <c r="Y136">
-        <v>606632211.5934989</v>
+        <v>1213264423.186998</v>
       </c>
       <c r="Z136">
-        <v>1898820148.55782</v>
+        <v>3797640297.11564</v>
       </c>
       <c r="AA136">
-        <v>5943499022.41125</v>
+        <v>11886998044.8225</v>
       </c>
       <c r="AB136">
-        <v>18603752786.2939</v>
+        <v>37207505572.5878</v>
       </c>
       <c r="AC136">
-        <v>58231626930.2803</v>
+        <v>116463253860.5606</v>
       </c>
       <c r="AD136">
-        <v>182270879101.639</v>
+        <v>364541758203.278</v>
       </c>
       <c r="AE136">
-        <v>570526277898.11</v>
+        <v>1141052555796.22</v>
       </c>
       <c r="AF136">
-        <v>1785804926034.09</v>
+        <v>3571609852068.18</v>
       </c>
       <c r="AG136">
-        <v>5589749950864.1</v>
+        <v>11179499901728.2</v>
       </c>
       <c r="AH136">
-        <v>17496482430796.4</v>
+        <v>34992964861592.8</v>
       </c>
       <c r="AI136">
-        <v>54765758780291.2</v>
+        <v>109531517560582.4</v>
       </c>
       <c r="AJ136">
-        <v>171422361417164</v>
+        <v>342844722834328</v>
       </c>
       <c r="AK136">
-        <v>536569320836505</v>
+        <v>1073138641673010</v>
       </c>
       <c r="AL136">
-        <v>1679516217620613</v>
+        <v>3359032435241226</v>
       </c>
       <c r="AM136">
-        <v>5257055548485508</v>
+        <v>1.051411109697102E+16</v>
       </c>
       <c r="AN136">
-        <v>1.64551153182762E+16</v>
+        <v>3.29102306365524E+16</v>
       </c>
       <c r="AO136">
-        <v>5.150617444317738E+16</v>
+        <v>1.030123488863548E+17</v>
       </c>
       <c r="AP136">
-        <v>1.612195329208381E+17</v>
+        <v>3.224390658416763E+17</v>
       </c>
       <c r="AQ136">
-        <v>5.04633436208465E+17</v>
+        <v>1.00926687241693E+18</v>
       </c>
       <c r="AR136">
-        <v>1.579553670240462E+18</v>
+        <v>3.159107340480924E+18</v>
       </c>
       <c r="AS136">
-        <v>4.944162669671833E+18</v>
+        <v>9.888325339343665E+18</v>
       </c>
     </row>
     <row r="137" spans="1:45">
@@ -17817,112 +17817,112 @@
         <v>1</v>
       </c>
       <c r="J138">
-        <v>206236223.839276</v>
+        <v>226859846.2232036</v>
       </c>
       <c r="K138">
-        <v>173289257.239228</v>
+        <v>190618182.9631508</v>
       </c>
       <c r="L138">
-        <v>144462465.731487</v>
+        <v>158908712.3046357</v>
       </c>
       <c r="M138">
-        <v>153234469.511311</v>
+        <v>168557916.4624421</v>
       </c>
       <c r="N138">
-        <v>149383278.142362</v>
+        <v>164321605.9565982</v>
       </c>
       <c r="O138">
-        <v>139177714.148699</v>
+        <v>153095485.5635689</v>
       </c>
       <c r="P138">
-        <v>139177700</v>
+        <v>153095470</v>
       </c>
       <c r="Q138">
-        <v>149866929.555882</v>
+        <v>164853622.5114702</v>
       </c>
       <c r="R138">
-        <v>161377121.295349</v>
+        <v>177514833.4248839</v>
       </c>
       <c r="S138">
-        <v>173771327.368545</v>
+        <v>191148460.1053995</v>
       </c>
       <c r="T138">
-        <v>187117442.503891</v>
+        <v>205829186.7542801</v>
       </c>
       <c r="U138">
-        <v>201488575.931399</v>
+        <v>221637433.5245389</v>
       </c>
       <c r="V138">
-        <v>216963451.870708</v>
+        <v>238659797.0577788</v>
       </c>
       <c r="W138">
-        <v>233626840.777714</v>
+        <v>256989524.8554854</v>
       </c>
       <c r="X138">
-        <v>251570023.71211</v>
+        <v>276727026.083321</v>
       </c>
       <c r="Y138">
-        <v>270891292.369642</v>
+        <v>297980421.6066062</v>
       </c>
       <c r="Z138">
-        <v>291696487.518209</v>
+        <v>320866136.2700299</v>
       </c>
       <c r="AA138">
-        <v>314099578.787331</v>
+        <v>345509536.6660641</v>
       </c>
       <c r="AB138">
-        <v>338223288.987052</v>
+        <v>372045617.8857573</v>
       </c>
       <c r="AC138">
-        <v>364199766.376231</v>
+        <v>400619743.0138541</v>
       </c>
       <c r="AD138">
-        <v>392171308.562904</v>
+        <v>431388439.4191945</v>
       </c>
       <c r="AE138">
-        <v>422291142.002166</v>
+        <v>464520256.2023826</v>
       </c>
       <c r="AF138">
-        <v>454724261.361637</v>
+        <v>500196687.4978007</v>
       </c>
       <c r="AG138">
-        <v>489648333.352505</v>
+        <v>538613166.6877556</v>
       </c>
       <c r="AH138">
-        <v>527254669.977265</v>
+        <v>579980136.9749916</v>
       </c>
       <c r="AI138">
-        <v>567749276.525569</v>
+        <v>624524204.1781259</v>
       </c>
       <c r="AJ138">
-        <v>611353980.059021</v>
+        <v>672489378.0649232</v>
       </c>
       <c r="AK138">
-        <v>658307644.566718</v>
+        <v>724138409.0233898</v>
       </c>
       <c r="AL138">
-        <v>708867479.448065</v>
+        <v>779754227.3928716</v>
       </c>
       <c r="AM138">
-        <v>763310448.490662</v>
+        <v>839641493.3397282</v>
       </c>
       <c r="AN138">
-        <v>821934787.0615669</v>
+        <v>904128265.7677237</v>
       </c>
       <c r="AO138">
-        <v>885061635.823014</v>
+        <v>973567799.4053155</v>
       </c>
       <c r="AP138">
-        <v>953036799.92198</v>
+        <v>1048340479.914178</v>
       </c>
       <c r="AQ138">
-        <v>1026232643.29034</v>
+        <v>1128855907.619374</v>
       </c>
       <c r="AR138">
-        <v>1105050128.4325</v>
+        <v>1215555141.27575</v>
       </c>
       <c r="AS138">
-        <v>1189921012.87428</v>
+        <v>1308913114.161708</v>
       </c>
     </row>
     <row r="139" spans="1:45">

</xml_diff>